<commit_message>
added columns to results, changed wafer allocations
</commit_message>
<xml_diff>
--- a/instrument_definition_inputs.xlsx
+++ b/instrument_definition_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbryan/Documents/atlast-telescope/sens_calc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369462C2-3225-A142-ACD3-6EEB6EEA916E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FD4C29-4BF5-F743-82B4-8C589A3A929F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="520" yWindow="1660" windowWidth="21240" windowHeight="11200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -363,7 +368,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,7 +455,7 @@
         <v>365</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>375</v>
@@ -464,7 +469,7 @@
         <v>420</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>375</v>
@@ -478,7 +483,7 @@
         <v>710</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>640</v>
@@ -492,7 +497,7 @@
         <v>900</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>870</v>

</xml_diff>

<commit_message>
more changed wafer allocations
</commit_message>
<xml_diff>
--- a/instrument_definition_inputs.xlsx
+++ b/instrument_definition_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbryan/Documents/atlast-telescope/sens_calc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93FD4C29-4BF5-F743-82B4-8C589A3A929F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463DF637-B9B5-6D45-8B89-3C57293494F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="1660" windowWidth="21240" windowHeight="11200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27340" yWindow="-10200" windowWidth="21240" windowHeight="11200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -399,7 +399,7 @@
         <v>110</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>120</v>
@@ -413,7 +413,7 @@
         <v>170</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>120</v>
@@ -427,7 +427,7 @@
         <v>245</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>250</v>
@@ -441,7 +441,7 @@
         <v>310</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>250</v>
@@ -455,7 +455,7 @@
         <v>365</v>
       </c>
       <c r="C6">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>375</v>
@@ -469,7 +469,7 @@
         <v>420</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>375</v>
@@ -497,7 +497,7 @@
         <v>900</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>870</v>
@@ -512,7 +512,7 @@
       </c>
       <c r="C10">
         <f>SUM(C2,C4,C6,C8,C9)</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
even more changed wafer allocations
</commit_message>
<xml_diff>
--- a/instrument_definition_inputs.xlsx
+++ b/instrument_definition_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbryan/Documents/atlast-telescope/sens_calc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463DF637-B9B5-6D45-8B89-3C57293494F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62677C44-AF8E-5A45-A9EA-99666857B0D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27340" yWindow="-10200" windowWidth="21240" windowHeight="11200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -368,7 +368,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,7 +455,7 @@
         <v>365</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>375</v>
@@ -469,7 +469,7 @@
         <v>420</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>375</v>
@@ -497,7 +497,7 @@
         <v>900</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>870</v>
@@ -512,7 +512,7 @@
       </c>
       <c r="C10">
         <f>SUM(C2,C4,C6,C8,C9)</f>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
initial edits to instrument input spreadsheet
</commit_message>
<xml_diff>
--- a/instrument_definition_inputs.xlsx
+++ b/instrument_definition_inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbryan/Documents/atlast-telescope/sens_calc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbryan/Documents/atlast-telescope/sens_calc_spec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348916C3-97DB-7648-9F50-48BCA372F3D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C3777D-1D97-C745-A477-6829C0118946}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27340" yWindow="-10200" windowWidth="21240" windowHeight="11200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41100" yWindow="-6920" windowWidth="21240" windowHeight="11200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>fmin</t>
   </si>
@@ -41,13 +41,10 @@
     <t>fmax</t>
   </si>
   <si>
-    <t>NaN</t>
+    <t>Nchan</t>
   </si>
   <si>
-    <t>Nwafer</t>
-  </si>
-  <si>
-    <t>det_spacing_freq</t>
+    <t>Nhorns</t>
   </si>
 </sst>
 </file>
@@ -365,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -385,137 +382,122 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>75</v>
+        <v>92.453749999999999</v>
       </c>
       <c r="B2">
-        <v>110</v>
+        <v>92.546250000000001</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>378</v>
       </c>
       <c r="D2">
-        <v>120</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>130</v>
+        <v>149.92500000000001</v>
       </c>
       <c r="B3">
-        <v>170</v>
+        <v>150.07499999999999</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>266</v>
       </c>
       <c r="D3">
-        <v>120</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>195</v>
+        <v>219.89</v>
       </c>
       <c r="B4">
-        <v>245</v>
+        <v>220.11</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>227</v>
       </c>
       <c r="D4">
-        <v>250</v>
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>245</v>
+        <v>277.36124999999998</v>
       </c>
       <c r="B5">
-        <v>310</v>
+        <v>277.63875000000002</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>234</v>
       </c>
       <c r="D5">
-        <v>250</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>335</v>
+        <v>349.82499999999999</v>
       </c>
       <c r="B6">
-        <v>365</v>
+        <v>350.17500000000001</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="D6">
-        <v>375</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>390</v>
+        <v>404.79750000000001</v>
       </c>
       <c r="B7">
-        <v>420</v>
+        <v>405.20249999999999</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="D7">
-        <v>375</v>
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>625</v>
+        <v>667.16624999999999</v>
       </c>
       <c r="B8">
-        <v>710</v>
+        <v>667.83375000000001</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>127</v>
       </c>
       <c r="D8">
-        <v>640</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>845</v>
+        <v>872.06375000000003</v>
       </c>
       <c r="B9">
-        <v>900</v>
+        <v>872.93624999999997</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="D9">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <f>SUM(C2,C4,C6,C8,C9)</f>
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>